<commit_message>
latest MOM and changes
</commit_message>
<xml_diff>
--- a/00_Financial project/CTSH.xlsx
+++ b/00_Financial project/CTSH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\04 - Semester4\03 - Financial Analytics\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\04 - Semester4\01 - capstone\Github\Capstone-Project\00_Financial project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CFAADF-8A0C-49C3-BA47-7966E5DE41AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2293DDA-F45B-4FFD-84C4-2B166F90672D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CTSH_MonteCarlo" sheetId="1" r:id="rId1"/>
@@ -2176,8 +2176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:P12"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="O89" sqref="O89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="M1" s="2">
         <f ca="1">I252</f>
-        <v>87.425698142927601</v>
+        <v>87.658193464810367</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.4">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="I2" s="18">
         <f ca="1">B2*EXP($F$5+$F$4*NORMSINV(RAND()))</f>
-        <v>56.467025510631004</v>
+        <v>57.547049621459749</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="I3" s="20">
         <f t="shared" ref="I3:I66" ca="1" si="1">B3*EXP($F$5+$F$4*NORMSINV(RAND()))</f>
-        <v>56.618974179207861</v>
+        <v>57.417580014612007</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="I4" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>55.766980119060598</v>
+        <v>56.367767170942088</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="I5" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.068247454528688</v>
+        <v>55.789396052220241</v>
       </c>
       <c r="L5">
         <f>L4+1</f>
@@ -2343,7 +2343,7 @@
       </c>
       <c r="I6" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>55.626930386595909</v>
+        <v>55.988345047931709</v>
       </c>
       <c r="L6">
         <f t="shared" ref="L6:L69" si="2">L5+1</f>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="I7" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>55.544368830178946</v>
+        <v>55.026956211219783</v>
       </c>
       <c r="L7">
         <f t="shared" si="2"/>
@@ -2389,7 +2389,7 @@
       </c>
       <c r="I8" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>56.077102740188273</v>
+        <v>55.755868367802826</v>
       </c>
       <c r="L8">
         <f t="shared" si="2"/>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="I9" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>53.062791906338795</v>
+        <v>57.118683651973505</v>
       </c>
       <c r="L9">
         <f t="shared" si="2"/>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="I10" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.220194524698094</v>
+        <v>54.876003959865422</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="I11" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>54.404920759864254</v>
+        <v>57.79758620650103</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="I12" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.087675615889154</v>
+        <v>56.072165898634289</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
@@ -2504,7 +2504,7 @@
       </c>
       <c r="I13" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>55.890971650495544</v>
+        <v>59.880609365943101</v>
       </c>
       <c r="L13">
         <f t="shared" si="2"/>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="I14" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>59.82561987592441</v>
+        <v>58.180344736649474</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="I15" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.584742641520222</v>
+        <v>60.372557916436982</v>
       </c>
       <c r="L15">
         <f t="shared" si="2"/>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="I16" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>56.88482204048546</v>
+        <v>58.198818513933062</v>
       </c>
       <c r="L16">
         <f t="shared" si="2"/>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="I17" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.683080074060342</v>
+        <v>56.142698668311738</v>
       </c>
       <c r="L17">
         <f t="shared" si="2"/>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="I18" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.826115641134358</v>
+        <v>58.318768248029123</v>
       </c>
       <c r="L18">
         <f t="shared" si="2"/>
@@ -2642,7 +2642,7 @@
       </c>
       <c r="I19" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.991286097106425</v>
+        <v>59.357266449007327</v>
       </c>
       <c r="L19">
         <f t="shared" si="2"/>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="I20" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>59.485319566391269</v>
+        <v>61.715904959683023</v>
       </c>
       <c r="L20">
         <f t="shared" si="2"/>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="I21" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>61.659628954034403</v>
+        <v>61.494968756065774</v>
       </c>
       <c r="L21">
         <f t="shared" si="2"/>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="I22" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>64.304085667912716</v>
+        <v>63.251083761207191</v>
       </c>
       <c r="L22">
         <f t="shared" si="2"/>
@@ -2734,7 +2734,7 @@
       </c>
       <c r="I23" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>61.263717100083817</v>
+        <v>61.472727520582609</v>
       </c>
       <c r="L23">
         <f t="shared" si="2"/>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="I24" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.30797134031782</v>
+        <v>59.478102002666532</v>
       </c>
       <c r="L24">
         <f t="shared" si="2"/>
@@ -2780,7 +2780,7 @@
       </c>
       <c r="I25" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>61.100238844474923</v>
+        <v>59.462084048697349</v>
       </c>
       <c r="L25">
         <f t="shared" si="2"/>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="I26" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.719582638847406</v>
+        <v>60.162366554174838</v>
       </c>
       <c r="L26">
         <f t="shared" si="2"/>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="I27" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.038166975050999</v>
+        <v>57.829346324076411</v>
       </c>
       <c r="L27">
         <f t="shared" si="2"/>
@@ -2849,7 +2849,7 @@
       </c>
       <c r="I28" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.874307356115885</v>
+        <v>58.880659268700931</v>
       </c>
       <c r="L28">
         <f t="shared" si="2"/>
@@ -2872,7 +2872,7 @@
       </c>
       <c r="I29" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>54.495369527605206</v>
+        <v>59.069704399477395</v>
       </c>
       <c r="L29">
         <f t="shared" si="2"/>
@@ -2895,7 +2895,7 @@
       </c>
       <c r="I30" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.547116994713036</v>
+        <v>60.852350185946385</v>
       </c>
       <c r="L30">
         <f t="shared" si="2"/>
@@ -2918,7 +2918,7 @@
       </c>
       <c r="I31" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.09386735889791</v>
+        <v>57.507960268295093</v>
       </c>
       <c r="L31">
         <f t="shared" si="2"/>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="I32" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.278168342952711</v>
+        <v>59.90417476801894</v>
       </c>
       <c r="L32">
         <f t="shared" si="2"/>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="I33" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>62.155381522722067</v>
+        <v>59.39944394514194</v>
       </c>
       <c r="L33">
         <f t="shared" si="2"/>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="I34" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.419017910615899</v>
+        <v>58.25150326908237</v>
       </c>
       <c r="L34">
         <f t="shared" si="2"/>
@@ -3010,7 +3010,7 @@
       </c>
       <c r="I35" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>56.208196835752929</v>
+        <v>57.942252798397682</v>
       </c>
       <c r="L35">
         <f t="shared" si="2"/>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="I36" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>56.908606301870883</v>
+        <v>59.632715272000603</v>
       </c>
       <c r="L36">
         <f t="shared" si="2"/>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="I37" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>54.21393017009138</v>
+        <v>53.345281222141573</v>
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
@@ -3079,7 +3079,7 @@
       </c>
       <c r="I38" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>54.789857126080911</v>
+        <v>54.498127967424672</v>
       </c>
       <c r="L38">
         <f t="shared" si="2"/>
@@ -3102,7 +3102,7 @@
       </c>
       <c r="I39" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>53.0241393605179</v>
+        <v>52.834496015117018</v>
       </c>
       <c r="L39">
         <f t="shared" si="2"/>
@@ -3125,7 +3125,7 @@
       </c>
       <c r="I40" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>54.727126065757744</v>
+        <v>52.064961598224919</v>
       </c>
       <c r="L40">
         <f t="shared" si="2"/>
@@ -3148,7 +3148,7 @@
       </c>
       <c r="I41" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>53.216248180235361</v>
+        <v>51.577503862198199</v>
       </c>
       <c r="L41">
         <f t="shared" si="2"/>
@@ -3171,7 +3171,7 @@
       </c>
       <c r="I42" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.357802623862284</v>
+        <v>59.89157512096979</v>
       </c>
       <c r="L42">
         <f t="shared" si="2"/>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="I43" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.936069561373635</v>
+        <v>61.579390975085332</v>
       </c>
       <c r="L43">
         <f t="shared" si="2"/>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="I44" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>62.837975067718247</v>
+        <v>58.872254983151841</v>
       </c>
       <c r="L44">
         <f t="shared" si="2"/>
@@ -3240,7 +3240,7 @@
       </c>
       <c r="I45" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>62.611480736345726</v>
+        <v>61.721634894371988</v>
       </c>
       <c r="L45">
         <f t="shared" si="2"/>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="I46" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>61.983322409518003</v>
+        <v>60.814971998545452</v>
       </c>
       <c r="L46">
         <f t="shared" si="2"/>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="I47" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>59.578870854361803</v>
+        <v>60.120672197185925</v>
       </c>
       <c r="L47">
         <f t="shared" si="2"/>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="I48" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.046188225600474</v>
+        <v>61.11032027506392</v>
       </c>
       <c r="L48">
         <f t="shared" si="2"/>
@@ -3332,7 +3332,7 @@
       </c>
       <c r="I49" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.988278724939413</v>
+        <v>58.997575399910538</v>
       </c>
       <c r="L49">
         <f t="shared" si="2"/>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="I50" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.433701023545403</v>
+        <v>61.832299298862885</v>
       </c>
       <c r="L50">
         <f t="shared" si="2"/>
@@ -3378,7 +3378,7 @@
       </c>
       <c r="I51" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.286827485160067</v>
+        <v>59.68147782524256</v>
       </c>
       <c r="L51">
         <f t="shared" si="2"/>
@@ -3401,7 +3401,7 @@
       </c>
       <c r="I52" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>59.019303683851696</v>
+        <v>58.817186074971076</v>
       </c>
       <c r="L52">
         <f t="shared" si="2"/>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="I53" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>60.393763354026937</v>
+        <v>60.687204254625271</v>
       </c>
       <c r="L53">
         <f t="shared" si="2"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="I54" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.235511068173977</v>
+        <v>58.232081490676748</v>
       </c>
       <c r="L54">
         <f t="shared" si="2"/>
@@ -3470,7 +3470,7 @@
       </c>
       <c r="I55" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>59.805447243725176</v>
+        <v>57.575910421899529</v>
       </c>
       <c r="L55">
         <f t="shared" si="2"/>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="I56" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>59.026886795726547</v>
+        <v>56.366957043864261</v>
       </c>
       <c r="L56">
         <f t="shared" si="2"/>
@@ -3516,7 +3516,7 @@
       </c>
       <c r="I57" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>56.013147368620473</v>
+        <v>56.925092082229703</v>
       </c>
       <c r="L57">
         <f t="shared" si="2"/>
@@ -3539,7 +3539,7 @@
       </c>
       <c r="I58" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.254155011223041</v>
+        <v>57.082770773293596</v>
       </c>
       <c r="L58">
         <f t="shared" si="2"/>
@@ -3562,7 +3562,7 @@
       </c>
       <c r="I59" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>61.053537681785947</v>
+        <v>58.718361456472337</v>
       </c>
       <c r="L59">
         <f t="shared" si="2"/>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="I60" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.585556007972848</v>
+        <v>56.455420479711499</v>
       </c>
       <c r="L60">
         <f t="shared" si="2"/>
@@ -3608,7 +3608,7 @@
       </c>
       <c r="I61" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>59.165759522021652</v>
+        <v>58.677975094754238</v>
       </c>
       <c r="L61">
         <f t="shared" si="2"/>
@@ -3631,7 +3631,7 @@
       </c>
       <c r="I62" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>59.223422944081278</v>
+        <v>59.363935081591912</v>
       </c>
       <c r="L62">
         <f t="shared" si="2"/>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="I63" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>61.46687062184877</v>
+        <v>59.350100108116834</v>
       </c>
       <c r="L63">
         <f t="shared" si="2"/>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="I64" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>57.094393191086887</v>
+        <v>60.864320437902393</v>
       </c>
       <c r="L64">
         <f t="shared" si="2"/>
@@ -3700,7 +3700,7 @@
       </c>
       <c r="I65" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>56.304171380746077</v>
+        <v>56.20127185012182</v>
       </c>
       <c r="L65">
         <f t="shared" si="2"/>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="I66" s="20">
         <f t="shared" ca="1" si="1"/>
-        <v>58.046615618664717</v>
+        <v>58.083554829903292</v>
       </c>
       <c r="L66">
         <f t="shared" si="2"/>
@@ -3746,7 +3746,7 @@
       </c>
       <c r="I67" s="20">
         <f t="shared" ref="I67:I130" ca="1" si="4">B67*EXP($F$5+$F$4*NORMSINV(RAND()))</f>
-        <v>59.864823538405993</v>
+        <v>59.431815100517163</v>
       </c>
       <c r="L67">
         <f t="shared" si="2"/>
@@ -3769,7 +3769,7 @@
       </c>
       <c r="I68" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>57.872439665666477</v>
+        <v>56.089507690301467</v>
       </c>
       <c r="L68">
         <f t="shared" si="2"/>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="I69" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>57.286743014075569</v>
+        <v>55.353914664795539</v>
       </c>
       <c r="L69">
         <f t="shared" si="2"/>
@@ -3815,7 +3815,7 @@
       </c>
       <c r="I70" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>57.536668932418202</v>
+        <v>58.031253423088124</v>
       </c>
       <c r="L70">
         <f t="shared" ref="L70:L133" si="5">L69+1</f>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="I71" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>58.883555242068809</v>
+        <v>61.372224095222151</v>
       </c>
       <c r="L71">
         <f t="shared" si="5"/>
@@ -3861,7 +3861,7 @@
       </c>
       <c r="I72" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>59.264661685848488</v>
+        <v>59.97069779557868</v>
       </c>
       <c r="L72">
         <f t="shared" si="5"/>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="I73" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>59.877807082795094</v>
+        <v>64.048459665000649</v>
       </c>
       <c r="L73">
         <f t="shared" si="5"/>
@@ -3907,7 +3907,7 @@
       </c>
       <c r="I74" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>62.296745065273548</v>
+        <v>60.594733411255916</v>
       </c>
       <c r="L74">
         <f t="shared" si="5"/>
@@ -3930,7 +3930,7 @@
       </c>
       <c r="I75" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>60.952589921984703</v>
+        <v>61.778703541806131</v>
       </c>
       <c r="L75">
         <f t="shared" si="5"/>
@@ -3953,7 +3953,7 @@
       </c>
       <c r="I76" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>59.849286057165905</v>
+        <v>61.717972290514744</v>
       </c>
       <c r="L76">
         <f t="shared" si="5"/>
@@ -3976,7 +3976,7 @@
       </c>
       <c r="I77" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>59.837173477303551</v>
+        <v>59.09217140262367</v>
       </c>
       <c r="L77">
         <f t="shared" si="5"/>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="I78" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>61.533025612468698</v>
+        <v>62.812672291380544</v>
       </c>
       <c r="L78">
         <f t="shared" si="5"/>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="I79" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.285566618675119</v>
+        <v>67.532385729432107</v>
       </c>
       <c r="L79">
         <f t="shared" si="5"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="I80" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>64.145701768404081</v>
+        <v>65.277031659171158</v>
       </c>
       <c r="L80">
         <f t="shared" si="5"/>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="I81" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.68015266710384</v>
+        <v>63.213332980366587</v>
       </c>
       <c r="L81">
         <f t="shared" si="5"/>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="I82" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>60.97947459478798</v>
+        <v>61.038220907946723</v>
       </c>
       <c r="L82">
         <f t="shared" si="5"/>
@@ -4114,7 +4114,7 @@
       </c>
       <c r="I83" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>60.583873530247608</v>
+        <v>61.402866358566804</v>
       </c>
       <c r="L83">
         <f t="shared" si="5"/>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="I84" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>61.86656615884462</v>
+        <v>64.158265610579633</v>
       </c>
       <c r="L84">
         <f t="shared" si="5"/>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="I85" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>64.497478634798441</v>
+        <v>60.271225054120187</v>
       </c>
       <c r="L85">
         <f t="shared" si="5"/>
@@ -4183,7 +4183,7 @@
       </c>
       <c r="I86" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>62.106954106367311</v>
+        <v>63.042871906924248</v>
       </c>
       <c r="L86">
         <f t="shared" si="5"/>
@@ -4206,7 +4206,7 @@
       </c>
       <c r="I87" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>64.505488146927178</v>
+        <v>65.055280775265757</v>
       </c>
       <c r="L87">
         <f t="shared" si="5"/>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="I88" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>62.335830182059865</v>
+        <v>62.428099051339402</v>
       </c>
       <c r="L88">
         <f t="shared" si="5"/>
@@ -4252,7 +4252,7 @@
       </c>
       <c r="I89" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.532076467593626</v>
+        <v>64.194684635152043</v>
       </c>
       <c r="L89">
         <f t="shared" si="5"/>
@@ -4275,7 +4275,7 @@
       </c>
       <c r="I90" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.458593124155655</v>
+        <v>67.518973759470029</v>
       </c>
       <c r="L90">
         <f t="shared" si="5"/>
@@ -4298,7 +4298,7 @@
       </c>
       <c r="I91" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.522054347570432</v>
+        <v>65.504406875593318</v>
       </c>
       <c r="L91">
         <f t="shared" si="5"/>
@@ -4321,7 +4321,7 @@
       </c>
       <c r="I92" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>64.396727633529693</v>
+        <v>65.261859657705173</v>
       </c>
       <c r="L92">
         <f t="shared" si="5"/>
@@ -4344,7 +4344,7 @@
       </c>
       <c r="I93" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.967746135891005</v>
+        <v>63.874813489806151</v>
       </c>
       <c r="L93">
         <f t="shared" si="5"/>
@@ -4367,7 +4367,7 @@
       </c>
       <c r="I94" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>67.825647670827621</v>
+        <v>64.131846086099742</v>
       </c>
       <c r="L94">
         <f t="shared" si="5"/>
@@ -4390,7 +4390,7 @@
       </c>
       <c r="I95" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.874661393747573</v>
+        <v>69.196454867189004</v>
       </c>
       <c r="L95">
         <f t="shared" si="5"/>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="I96" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>69.473007438732253</v>
+        <v>67.739301103659855</v>
       </c>
       <c r="L96">
         <f t="shared" si="5"/>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="I97" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>69.73668773923221</v>
+        <v>71.158226855235228</v>
       </c>
       <c r="L97">
         <f t="shared" si="5"/>
@@ -4459,7 +4459,7 @@
       </c>
       <c r="I98" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>70.333891415014079</v>
+        <v>68.253286154711361</v>
       </c>
       <c r="L98">
         <f t="shared" si="5"/>
@@ -4482,7 +4482,7 @@
       </c>
       <c r="I99" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>69.833742557677596</v>
+        <v>67.226778102838779</v>
       </c>
       <c r="L99">
         <f t="shared" si="5"/>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="I100" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>67.867145406606099</v>
+        <v>65.131359363826206</v>
       </c>
       <c r="L100">
         <f t="shared" si="5"/>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="I101" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>70.560694281019252</v>
+        <v>69.884292526195495</v>
       </c>
       <c r="L101">
         <f t="shared" si="5"/>
@@ -4551,7 +4551,7 @@
       </c>
       <c r="I102" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>67.127236375168025</v>
+        <v>66.159470989439811</v>
       </c>
       <c r="L102">
         <f t="shared" si="5"/>
@@ -4574,7 +4574,7 @@
       </c>
       <c r="I103" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.594238067219706</v>
+        <v>67.083258920349252</v>
       </c>
       <c r="L103">
         <f t="shared" si="5"/>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="I104" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>66.947614108602366</v>
+        <v>68.561866697054043</v>
       </c>
       <c r="L104">
         <f t="shared" si="5"/>
@@ -4620,7 +4620,7 @@
       </c>
       <c r="I105" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>66.667630829834195</v>
+        <v>64.75053581789409</v>
       </c>
       <c r="L105">
         <f t="shared" si="5"/>
@@ -4643,7 +4643,7 @@
       </c>
       <c r="I106" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>67.420859556091088</v>
+        <v>71.02800492156878</v>
       </c>
       <c r="L106">
         <f t="shared" si="5"/>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="I107" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>67.440018265568071</v>
+        <v>66.75663367054257</v>
       </c>
       <c r="L107">
         <f t="shared" si="5"/>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="I108" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.691199436848422</v>
+        <v>66.614516539139117</v>
       </c>
       <c r="L108">
         <f t="shared" si="5"/>
@@ -4712,7 +4712,7 @@
       </c>
       <c r="I109" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>63.39018327251938</v>
+        <v>66.921785084904656</v>
       </c>
       <c r="L109">
         <f t="shared" si="5"/>
@@ -4735,7 +4735,7 @@
       </c>
       <c r="I110" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>66.363574021873049</v>
+        <v>67.341821621787162</v>
       </c>
       <c r="L110">
         <f t="shared" si="5"/>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="I111" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>68.473879131094336</v>
+        <v>70.697371157620552</v>
       </c>
       <c r="L111">
         <f t="shared" si="5"/>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="I112" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>63.079871949070501</v>
+        <v>66.750313247521177</v>
       </c>
       <c r="L112">
         <f t="shared" si="5"/>
@@ -4804,7 +4804,7 @@
       </c>
       <c r="I113" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>68.212390822607148</v>
+        <v>67.448587170754806</v>
       </c>
       <c r="L113">
         <f t="shared" si="5"/>
@@ -4827,7 +4827,7 @@
       </c>
       <c r="I114" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>66.178157044090298</v>
+        <v>68.880803197836173</v>
       </c>
       <c r="L114">
         <f t="shared" si="5"/>
@@ -4850,7 +4850,7 @@
       </c>
       <c r="I115" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>68.751814519252335</v>
+        <v>67.909271332117498</v>
       </c>
       <c r="L115">
         <f t="shared" si="5"/>
@@ -4873,7 +4873,7 @@
       </c>
       <c r="I116" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>67.173840936774198</v>
+        <v>65.462328295089378</v>
       </c>
       <c r="L116">
         <f t="shared" si="5"/>
@@ -4896,7 +4896,7 @@
       </c>
       <c r="I117" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>68.12585992523033</v>
+        <v>67.828638904536334</v>
       </c>
       <c r="L117">
         <f t="shared" si="5"/>
@@ -4919,7 +4919,7 @@
       </c>
       <c r="I118" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>63.567746602921154</v>
+        <v>63.245921340190243</v>
       </c>
       <c r="L118">
         <f t="shared" si="5"/>
@@ -4942,7 +4942,7 @@
       </c>
       <c r="I119" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.130179773222082</v>
+        <v>63.210686062189325</v>
       </c>
       <c r="L119">
         <f t="shared" si="5"/>
@@ -4965,7 +4965,7 @@
       </c>
       <c r="I120" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.062592553043444</v>
+        <v>62.881700000609548</v>
       </c>
       <c r="L120">
         <f t="shared" si="5"/>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="I121" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>63.92717878538447</v>
+        <v>63.446612459990398</v>
       </c>
       <c r="L121">
         <f t="shared" si="5"/>
@@ -5011,7 +5011,7 @@
       </c>
       <c r="I122" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.746713972235582</v>
+        <v>63.923742909852713</v>
       </c>
       <c r="L122">
         <f t="shared" si="5"/>
@@ -5034,7 +5034,7 @@
       </c>
       <c r="I123" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>64.707073192588993</v>
+        <v>66.196390950097054</v>
       </c>
       <c r="L123">
         <f t="shared" si="5"/>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="I124" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>66.925926326589746</v>
+        <v>65.600155913409594</v>
       </c>
       <c r="L124">
         <f t="shared" si="5"/>
@@ -5080,7 +5080,7 @@
       </c>
       <c r="I125" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>68.046482840251443</v>
+        <v>63.589129119128351</v>
       </c>
       <c r="L125">
         <f t="shared" si="5"/>
@@ -5103,7 +5103,7 @@
       </c>
       <c r="I126" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>65.833649361755533</v>
+        <v>67.877362386467226</v>
       </c>
       <c r="L126">
         <f t="shared" si="5"/>
@@ -5126,7 +5126,7 @@
       </c>
       <c r="I127" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>64.306055104040595</v>
+        <v>65.27962628567289</v>
       </c>
       <c r="L127">
         <f t="shared" si="5"/>
@@ -5149,7 +5149,7 @@
       </c>
       <c r="I128" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>68.106752039317456</v>
+        <v>66.424494258342534</v>
       </c>
       <c r="L128">
         <f t="shared" si="5"/>
@@ -5172,7 +5172,7 @@
       </c>
       <c r="I129" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>66.164105473041872</v>
+        <v>67.356367647957541</v>
       </c>
       <c r="L129">
         <f t="shared" si="5"/>
@@ -5195,7 +5195,7 @@
       </c>
       <c r="I130" s="20">
         <f t="shared" ca="1" si="4"/>
-        <v>67.452911398067911</v>
+        <v>68.223409230043046</v>
       </c>
       <c r="L130">
         <f t="shared" si="5"/>
@@ -5218,7 +5218,7 @@
       </c>
       <c r="I131" s="20">
         <f t="shared" ref="I131:I194" ca="1" si="7">B131*EXP($F$5+$F$4*NORMSINV(RAND()))</f>
-        <v>65.90404789447966</v>
+        <v>68.153794717788315</v>
       </c>
       <c r="L131">
         <f t="shared" si="5"/>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="I132" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>68.972984252800927</v>
+        <v>69.495215586881429</v>
       </c>
       <c r="L132">
         <f t="shared" si="5"/>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="I133" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>67.569968265929461</v>
+        <v>68.392586273185742</v>
       </c>
       <c r="L133">
         <f t="shared" si="5"/>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="I134" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>68.36842595721069</v>
+        <v>66.439106492249948</v>
       </c>
       <c r="L134">
         <f t="shared" ref="L134:L197" si="8">L133+1</f>
@@ -5310,7 +5310,7 @@
       </c>
       <c r="I135" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>62.473078792799662</v>
+        <v>65.630520007998925</v>
       </c>
       <c r="L135">
         <f t="shared" si="8"/>
@@ -5333,7 +5333,7 @@
       </c>
       <c r="I136" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>67.887056925727109</v>
+        <v>68.966997145549612</v>
       </c>
       <c r="L136">
         <f t="shared" si="8"/>
@@ -5356,7 +5356,7 @@
       </c>
       <c r="I137" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>67.553975171270764</v>
+        <v>65.351831028796397</v>
       </c>
       <c r="L137">
         <f t="shared" si="8"/>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="I138" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>66.52508399389427</v>
+        <v>65.421673903719466</v>
       </c>
       <c r="L138">
         <f t="shared" si="8"/>
@@ -5402,7 +5402,7 @@
       </c>
       <c r="I139" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>66.59365945365677</v>
+        <v>65.567729635251482</v>
       </c>
       <c r="L139">
         <f t="shared" si="8"/>
@@ -5425,7 +5425,7 @@
       </c>
       <c r="I140" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>64.587732580599635</v>
+        <v>67.677324094299109</v>
       </c>
       <c r="L140">
         <f t="shared" si="8"/>
@@ -5448,7 +5448,7 @@
       </c>
       <c r="I141" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>66.355254979827194</v>
+        <v>67.160343658062502</v>
       </c>
       <c r="L141">
         <f t="shared" si="8"/>
@@ -5471,7 +5471,7 @@
       </c>
       <c r="I142" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>70.787043889326824</v>
+        <v>70.898118434064429</v>
       </c>
       <c r="L142">
         <f t="shared" si="8"/>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="I143" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>68.925222890414574</v>
+        <v>72.545006300240857</v>
       </c>
       <c r="L143">
         <f t="shared" si="8"/>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="I144" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>68.80501247272305</v>
+        <v>68.310039501268037</v>
       </c>
       <c r="L144">
         <f t="shared" si="8"/>
@@ -5540,7 +5540,7 @@
       </c>
       <c r="I145" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>74.275598028113151</v>
+        <v>74.134789804066827</v>
       </c>
       <c r="L145">
         <f t="shared" si="8"/>
@@ -5563,7 +5563,7 @@
       </c>
       <c r="I146" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>71.999209015637661</v>
+        <v>73.832346065641232</v>
       </c>
       <c r="L146">
         <f t="shared" si="8"/>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="I147" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>71.980212139448597</v>
+        <v>74.723141030490282</v>
       </c>
       <c r="L147">
         <f t="shared" si="8"/>
@@ -5609,7 +5609,7 @@
       </c>
       <c r="I148" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>74.561010501078826</v>
+        <v>74.257418815391546</v>
       </c>
       <c r="L148">
         <f t="shared" si="8"/>
@@ -5632,7 +5632,7 @@
       </c>
       <c r="I149" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>72.999610442128827</v>
+        <v>71.855630724629918</v>
       </c>
       <c r="L149">
         <f t="shared" si="8"/>
@@ -5655,7 +5655,7 @@
       </c>
       <c r="I150" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>73.102328368065784</v>
+        <v>70.61111616530475</v>
       </c>
       <c r="L150">
         <f t="shared" si="8"/>
@@ -5678,7 +5678,7 @@
       </c>
       <c r="I151" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>73.5033329939358</v>
+        <v>73.487609154827169</v>
       </c>
       <c r="L151">
         <f t="shared" si="8"/>
@@ -5701,7 +5701,7 @@
       </c>
       <c r="I152" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>72.359547015196299</v>
+        <v>72.022502417702455</v>
       </c>
       <c r="L152">
         <f t="shared" si="8"/>
@@ -5724,7 +5724,7 @@
       </c>
       <c r="I153" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>69.965480068721106</v>
+        <v>68.630190367705424</v>
       </c>
       <c r="L153">
         <f t="shared" si="8"/>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="I154" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>66.755720247659738</v>
+        <v>68.449041753945423</v>
       </c>
       <c r="L154">
         <f t="shared" si="8"/>
@@ -5770,7 +5770,7 @@
       </c>
       <c r="I155" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>69.344389256888974</v>
+        <v>73.050738839243948</v>
       </c>
       <c r="L155">
         <f t="shared" si="8"/>
@@ -5793,7 +5793,7 @@
       </c>
       <c r="I156" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>67.153852634933543</v>
+        <v>67.62821521578492</v>
       </c>
       <c r="L156">
         <f t="shared" si="8"/>
@@ -5816,7 +5816,7 @@
       </c>
       <c r="I157" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>65.592972765437494</v>
+        <v>68.742421965029735</v>
       </c>
       <c r="L157">
         <f t="shared" si="8"/>
@@ -5839,7 +5839,7 @@
       </c>
       <c r="I158" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>69.487932584235296</v>
+        <v>67.504894318019751</v>
       </c>
       <c r="L158">
         <f t="shared" si="8"/>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="I159" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>74.932744080930007</v>
+        <v>72.634039664802245</v>
       </c>
       <c r="L159">
         <f t="shared" si="8"/>
@@ -5885,7 +5885,7 @@
       </c>
       <c r="I160" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>70.664646696337044</v>
+        <v>73.096803888544429</v>
       </c>
       <c r="L160">
         <f t="shared" si="8"/>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="I161" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>73.46417875119397</v>
+        <v>70.726743138814072</v>
       </c>
       <c r="L161">
         <f t="shared" si="8"/>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="I162" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>72.558285391859528</v>
+        <v>68.942083051861019</v>
       </c>
       <c r="L162">
         <f t="shared" si="8"/>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="I163" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>70.965203787867992</v>
+        <v>71.926756853591996</v>
       </c>
       <c r="L163">
         <f t="shared" si="8"/>
@@ -5977,7 +5977,7 @@
       </c>
       <c r="I164" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>70.878089179918931</v>
+        <v>73.59601839026908</v>
       </c>
       <c r="L164">
         <f t="shared" si="8"/>
@@ -6000,7 +6000,7 @@
       </c>
       <c r="I165" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>72.978383584557989</v>
+        <v>75.4936526828117</v>
       </c>
       <c r="L165">
         <f t="shared" si="8"/>
@@ -6023,7 +6023,7 @@
       </c>
       <c r="I166" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>71.669322626425739</v>
+        <v>73.702083384857659</v>
       </c>
       <c r="L166">
         <f t="shared" si="8"/>
@@ -6046,7 +6046,7 @@
       </c>
       <c r="I167" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>73.70125515749298</v>
+        <v>71.864758881180393</v>
       </c>
       <c r="L167">
         <f t="shared" si="8"/>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="I168" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>86.646799734727111</v>
+        <v>82.370110625610963</v>
       </c>
       <c r="L168">
         <f t="shared" si="8"/>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="I169" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>78.17706062608616</v>
+        <v>80.979619808488494</v>
       </c>
       <c r="L169">
         <f t="shared" si="8"/>
@@ -6115,7 +6115,7 @@
       </c>
       <c r="I170" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>79.771902395413363</v>
+        <v>77.548693875154825</v>
       </c>
       <c r="L170">
         <f t="shared" si="8"/>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="I171" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>82.738339502594854</v>
+        <v>79.752563867051336</v>
       </c>
       <c r="L171">
         <f t="shared" si="8"/>
@@ -6161,7 +6161,7 @@
       </c>
       <c r="I172" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>84.553336566655304</v>
+        <v>82.748103128213771</v>
       </c>
       <c r="L172">
         <f t="shared" si="8"/>
@@ -6184,7 +6184,7 @@
       </c>
       <c r="I173" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>81.661959934792122</v>
+        <v>80.507021783200059</v>
       </c>
       <c r="L173">
         <f t="shared" si="8"/>
@@ -6207,7 +6207,7 @@
       </c>
       <c r="I174" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>82.298560054311793</v>
+        <v>82.17169458555982</v>
       </c>
       <c r="L174">
         <f t="shared" si="8"/>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="I175" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>80.648642728422331</v>
+        <v>81.630386798817568</v>
       </c>
       <c r="L175">
         <f t="shared" si="8"/>
@@ -6253,7 +6253,7 @@
       </c>
       <c r="I176" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>81.410020805690991</v>
+        <v>82.862780701112939</v>
       </c>
       <c r="L176">
         <f t="shared" si="8"/>
@@ -6276,7 +6276,7 @@
       </c>
       <c r="I177" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>84.71560260931642</v>
+        <v>82.462829181635328</v>
       </c>
       <c r="L177">
         <f t="shared" si="8"/>
@@ -6299,7 +6299,7 @@
       </c>
       <c r="I178" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>84.282775416837055</v>
+        <v>83.891633009077495</v>
       </c>
       <c r="L178">
         <f t="shared" si="8"/>
@@ -6322,7 +6322,7 @@
       </c>
       <c r="I179" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>83.670043716718496</v>
+        <v>86.585346809237237</v>
       </c>
       <c r="L179">
         <f t="shared" si="8"/>
@@ -6345,7 +6345,7 @@
       </c>
       <c r="I180" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>82.948597399160803</v>
+        <v>84.069612686194503</v>
       </c>
       <c r="L180">
         <f t="shared" si="8"/>
@@ -6368,7 +6368,7 @@
       </c>
       <c r="I181" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>80.488472248567973</v>
+        <v>81.593089827649294</v>
       </c>
       <c r="L181">
         <f t="shared" si="8"/>
@@ -6391,7 +6391,7 @@
       </c>
       <c r="I182" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>84.667033759727701</v>
+        <v>81.852402043832015</v>
       </c>
       <c r="L182">
         <f t="shared" si="8"/>
@@ -6414,7 +6414,7 @@
       </c>
       <c r="I183" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>80.88220533572904</v>
+        <v>88.268770716322365</v>
       </c>
       <c r="L183">
         <f t="shared" si="8"/>
@@ -6437,7 +6437,7 @@
       </c>
       <c r="I184" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>85.184010141946544</v>
+        <v>84.443957041191467</v>
       </c>
       <c r="L184">
         <f t="shared" si="8"/>
@@ -6460,7 +6460,7 @@
       </c>
       <c r="I185" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>87.128193554353956</v>
+        <v>86.532320322128271</v>
       </c>
       <c r="L185">
         <f t="shared" si="8"/>
@@ -6483,7 +6483,7 @@
       </c>
       <c r="I186" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>88.24732871479722</v>
+        <v>83.538544430313735</v>
       </c>
       <c r="L186">
         <f t="shared" si="8"/>
@@ -6506,7 +6506,7 @@
       </c>
       <c r="I187" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>84.548558562946269</v>
+        <v>87.740157774139817</v>
       </c>
       <c r="L187">
         <f t="shared" si="8"/>
@@ -6529,7 +6529,7 @@
       </c>
       <c r="I188" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>85.404569493367205</v>
+        <v>86.820420440038887</v>
       </c>
       <c r="L188">
         <f t="shared" si="8"/>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="I189" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>86.199309571916871</v>
+        <v>89.924130699359367</v>
       </c>
       <c r="L189">
         <f t="shared" si="8"/>
@@ -6575,7 +6575,7 @@
       </c>
       <c r="I190" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>90.634578839923648</v>
+        <v>89.24147088373951</v>
       </c>
       <c r="L190">
         <f t="shared" si="8"/>
@@ -6598,7 +6598,7 @@
       </c>
       <c r="I191" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>85.872202499880927</v>
+        <v>87.479070969068403</v>
       </c>
       <c r="L191">
         <f t="shared" si="8"/>
@@ -6621,7 +6621,7 @@
       </c>
       <c r="I192" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>87.894788493979192</v>
+        <v>90.924506152663284</v>
       </c>
       <c r="L192">
         <f t="shared" si="8"/>
@@ -6644,7 +6644,7 @@
       </c>
       <c r="I193" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>90.652698904488616</v>
+        <v>90.553631754469762</v>
       </c>
       <c r="L193">
         <f t="shared" si="8"/>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="I194" s="20">
         <f t="shared" ca="1" si="7"/>
-        <v>86.890077923814729</v>
+        <v>88.545456708253866</v>
       </c>
       <c r="L194">
         <f t="shared" si="8"/>
@@ -6690,7 +6690,7 @@
       </c>
       <c r="I195" s="20">
         <f t="shared" ref="I195:I251" ca="1" si="10">B195*EXP($F$5+$F$4*NORMSINV(RAND()))</f>
-        <v>89.631942629059651</v>
+        <v>89.217316665587603</v>
       </c>
       <c r="L195">
         <f t="shared" si="8"/>
@@ -6713,7 +6713,7 @@
       </c>
       <c r="I196" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>89.083770382896034</v>
+        <v>86.765478456152039</v>
       </c>
       <c r="L196">
         <f t="shared" si="8"/>
@@ -6736,7 +6736,7 @@
       </c>
       <c r="I197" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>90.382638155173666</v>
+        <v>90.05126808844885</v>
       </c>
       <c r="L197">
         <f t="shared" si="8"/>
@@ -6759,7 +6759,7 @@
       </c>
       <c r="I198" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>91.042856458760923</v>
+        <v>93.877980710921108</v>
       </c>
       <c r="L198">
         <f t="shared" ref="L198:L261" si="11">L197+1</f>
@@ -6782,7 +6782,7 @@
       </c>
       <c r="I199" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.914782753319727</v>
+        <v>86.333184927615605</v>
       </c>
       <c r="L199">
         <f t="shared" si="11"/>
@@ -6805,7 +6805,7 @@
       </c>
       <c r="I200" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>92.484726360957652</v>
+        <v>90.55957245738486</v>
       </c>
       <c r="L200">
         <f t="shared" si="11"/>
@@ -6828,7 +6828,7 @@
       </c>
       <c r="I201" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>92.846851281486721</v>
+        <v>84.894797684807116</v>
       </c>
       <c r="L201">
         <f t="shared" si="11"/>
@@ -6851,7 +6851,7 @@
       </c>
       <c r="I202" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.110945719104237</v>
+        <v>86.053041780149854</v>
       </c>
       <c r="L202">
         <f t="shared" si="11"/>
@@ -6874,7 +6874,7 @@
       </c>
       <c r="I203" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>86.251785229975013</v>
+        <v>87.292074790349119</v>
       </c>
       <c r="L203">
         <f t="shared" si="11"/>
@@ -6897,7 +6897,7 @@
       </c>
       <c r="I204" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>84.563201100827442</v>
+        <v>84.575369042536693</v>
       </c>
       <c r="L204">
         <f t="shared" si="11"/>
@@ -6920,7 +6920,7 @@
       </c>
       <c r="I205" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>80.540413095736412</v>
+        <v>83.180441552696308</v>
       </c>
       <c r="L205">
         <f t="shared" si="11"/>
@@ -6943,7 +6943,7 @@
       </c>
       <c r="I206" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>86.430689469818248</v>
+        <v>89.612841548899212</v>
       </c>
       <c r="L206">
         <f t="shared" si="11"/>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="I207" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.330675732779582</v>
+        <v>86.646687085495202</v>
       </c>
       <c r="L207">
         <f t="shared" si="11"/>
@@ -6989,7 +6989,7 @@
       </c>
       <c r="I208" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>83.406404719070892</v>
+        <v>86.684478359749974</v>
       </c>
       <c r="L208">
         <f t="shared" si="11"/>
@@ -7012,7 +7012,7 @@
       </c>
       <c r="I209" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.504581910727211</v>
+        <v>84.178273722434781</v>
       </c>
       <c r="L209">
         <f t="shared" si="11"/>
@@ -7035,7 +7035,7 @@
       </c>
       <c r="I210" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.342185300066362</v>
+        <v>87.880601634468718</v>
       </c>
       <c r="L210">
         <f t="shared" si="11"/>
@@ -7058,7 +7058,7 @@
       </c>
       <c r="I211" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>84.875128929852153</v>
+        <v>89.417297152329041</v>
       </c>
       <c r="L211">
         <f t="shared" si="11"/>
@@ -7081,7 +7081,7 @@
       </c>
       <c r="I212" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.398425914369128</v>
+        <v>86.950305160602696</v>
       </c>
       <c r="L212">
         <f t="shared" si="11"/>
@@ -7104,7 +7104,7 @@
       </c>
       <c r="I213" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>81.788397402742845</v>
+        <v>85.433643740097295</v>
       </c>
       <c r="L213">
         <f t="shared" si="11"/>
@@ -7127,7 +7127,7 @@
       </c>
       <c r="I214" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.271538803718329</v>
+        <v>86.249015608822873</v>
       </c>
       <c r="L214">
         <f t="shared" si="11"/>
@@ -7150,7 +7150,7 @@
       </c>
       <c r="I215" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.693966722380097</v>
+        <v>87.786802846914441</v>
       </c>
       <c r="L215">
         <f t="shared" si="11"/>
@@ -7173,7 +7173,7 @@
       </c>
       <c r="I216" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>86.348070116993227</v>
+        <v>83.773525585900501</v>
       </c>
       <c r="L216">
         <f t="shared" si="11"/>
@@ -7196,7 +7196,7 @@
       </c>
       <c r="I217" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.548852098550583</v>
+        <v>80.323297493218817</v>
       </c>
       <c r="L217">
         <f t="shared" si="11"/>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="I218" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>83.640544023326967</v>
+        <v>79.041857007974968</v>
       </c>
       <c r="L218">
         <f t="shared" si="11"/>
@@ -7242,7 +7242,7 @@
       </c>
       <c r="I219" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>89.080513403794555</v>
+        <v>83.684470102578061</v>
       </c>
       <c r="L219">
         <f t="shared" si="11"/>
@@ -7265,7 +7265,7 @@
       </c>
       <c r="I220" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.422322059757917</v>
+        <v>84.720764978287448</v>
       </c>
       <c r="L220">
         <f t="shared" si="11"/>
@@ -7288,7 +7288,7 @@
       </c>
       <c r="I221" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.310980434138443</v>
+        <v>84.654070539533549</v>
       </c>
       <c r="L221">
         <f t="shared" si="11"/>
@@ -7311,7 +7311,7 @@
       </c>
       <c r="I222" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>86.93079250872843</v>
+        <v>89.218876485205769</v>
       </c>
       <c r="L222">
         <f t="shared" si="11"/>
@@ -7334,7 +7334,7 @@
       </c>
       <c r="I223" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>87.104271877999778</v>
+        <v>85.302653023354509</v>
       </c>
       <c r="L223">
         <f t="shared" si="11"/>
@@ -7357,7 +7357,7 @@
       </c>
       <c r="I224" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.372487895007112</v>
+        <v>85.385044927709586</v>
       </c>
       <c r="L224">
         <f t="shared" si="11"/>
@@ -7380,7 +7380,7 @@
       </c>
       <c r="I225" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.506551438475682</v>
+        <v>84.040921677723929</v>
       </c>
       <c r="L225">
         <f t="shared" si="11"/>
@@ -7403,7 +7403,7 @@
       </c>
       <c r="I226" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>90.64306665044505</v>
+        <v>89.61130846743454</v>
       </c>
       <c r="L226">
         <f t="shared" si="11"/>
@@ -7426,7 +7426,7 @@
       </c>
       <c r="I227" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>86.590310630797774</v>
+        <v>89.425530777423873</v>
       </c>
       <c r="L227">
         <f t="shared" si="11"/>
@@ -7449,7 +7449,7 @@
       </c>
       <c r="I228" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.458222893926049</v>
+        <v>87.366189977071301</v>
       </c>
       <c r="L228">
         <f t="shared" si="11"/>
@@ -7472,7 +7472,7 @@
       </c>
       <c r="I229" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>82.317830188535993</v>
+        <v>87.884293523392188</v>
       </c>
       <c r="L229">
         <f t="shared" si="11"/>
@@ -7495,7 +7495,7 @@
       </c>
       <c r="I230" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>84.948101684245927</v>
+        <v>83.203247846676589</v>
       </c>
       <c r="L230">
         <f t="shared" si="11"/>
@@ -7518,7 +7518,7 @@
       </c>
       <c r="I231" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>87.481975940042659</v>
+        <v>87.366887475991859</v>
       </c>
       <c r="L231">
         <f t="shared" si="11"/>
@@ -7541,7 +7541,7 @@
       </c>
       <c r="I232" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.530772581678448</v>
+        <v>84.173919683838122</v>
       </c>
       <c r="L232">
         <f t="shared" si="11"/>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="I233" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>87.515399037895747</v>
+        <v>85.198290298342371</v>
       </c>
       <c r="L233">
         <f t="shared" si="11"/>
@@ -7587,7 +7587,7 @@
       </c>
       <c r="I234" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>79.639597195857547</v>
+        <v>83.008643458656849</v>
       </c>
       <c r="L234">
         <f t="shared" si="11"/>
@@ -7610,7 +7610,7 @@
       </c>
       <c r="I235" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>83.917059538180027</v>
+        <v>79.190561915711626</v>
       </c>
       <c r="L235">
         <f t="shared" si="11"/>
@@ -7633,7 +7633,7 @@
       </c>
       <c r="I236" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>81.419191533376534</v>
+        <v>79.147227341651742</v>
       </c>
       <c r="L236">
         <f t="shared" si="11"/>
@@ -7656,7 +7656,7 @@
       </c>
       <c r="I237" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>81.495088379196901</v>
+        <v>81.599012811925348</v>
       </c>
       <c r="L237">
         <f t="shared" si="11"/>
@@ -7679,7 +7679,7 @@
       </c>
       <c r="I238" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>83.575858552609645</v>
+        <v>85.731424354783911</v>
       </c>
       <c r="L238">
         <f t="shared" si="11"/>
@@ -7702,7 +7702,7 @@
       </c>
       <c r="I239" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>85.377701043372838</v>
+        <v>81.075242918734205</v>
       </c>
       <c r="L239">
         <f t="shared" si="11"/>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="I240" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>87.489340169605597</v>
+        <v>84.025825575977777</v>
       </c>
       <c r="L240">
         <f t="shared" si="11"/>
@@ -7748,7 +7748,7 @@
       </c>
       <c r="I241" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>82.197252811587816</v>
+        <v>83.928306958315886</v>
       </c>
       <c r="L241">
         <f t="shared" si="11"/>
@@ -7771,7 +7771,7 @@
       </c>
       <c r="I242" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>84.75172763323323</v>
+        <v>80.927100280522154</v>
       </c>
       <c r="L242">
         <f t="shared" si="11"/>
@@ -7794,7 +7794,7 @@
       </c>
       <c r="I243" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>82.993188636704318</v>
+        <v>83.003715055698549</v>
       </c>
       <c r="L243">
         <f t="shared" si="11"/>
@@ -7817,7 +7817,7 @@
       </c>
       <c r="I244" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>84.38529626422222</v>
+        <v>87.702957770408631</v>
       </c>
       <c r="L244">
         <f t="shared" si="11"/>
@@ -7840,7 +7840,7 @@
       </c>
       <c r="I245" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.063897415036507</v>
+        <v>85.4816942823566</v>
       </c>
       <c r="L245">
         <f t="shared" si="11"/>
@@ -7863,7 +7863,7 @@
       </c>
       <c r="I246" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>87.153543293048216</v>
+        <v>87.676733724838613</v>
       </c>
       <c r="L246">
         <f t="shared" si="11"/>
@@ -7886,7 +7886,7 @@
       </c>
       <c r="I247" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>87.777110291707288</v>
+        <v>85.740492146843494</v>
       </c>
       <c r="L247">
         <f t="shared" si="11"/>
@@ -7909,7 +7909,7 @@
       </c>
       <c r="I248" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>83.48158357517346</v>
+        <v>83.211531604110576</v>
       </c>
       <c r="L248">
         <f t="shared" si="11"/>
@@ -7932,7 +7932,7 @@
       </c>
       <c r="I249" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>89.195944458994376</v>
+        <v>85.666272782504677</v>
       </c>
       <c r="L249">
         <f t="shared" si="11"/>
@@ -7955,7 +7955,7 @@
       </c>
       <c r="I250" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.246056047187537</v>
+        <v>85.172578435887303</v>
       </c>
       <c r="L250">
         <f t="shared" si="11"/>
@@ -7978,7 +7978,7 @@
       </c>
       <c r="I251" s="20">
         <f t="shared" ca="1" si="10"/>
-        <v>88.650979578086691</v>
+        <v>90.25777741407947</v>
       </c>
       <c r="L251">
         <f t="shared" si="11"/>
@@ -7998,7 +7998,7 @@
       </c>
       <c r="I252" s="22">
         <f ca="1">B252*EXP($F$5+$F$4*NORMSINV(RAND()))</f>
-        <v>87.425698142927601</v>
+        <v>87.658193464810367</v>
       </c>
       <c r="L252">
         <f t="shared" si="11"/>
@@ -66728,8 +66728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2786E0E5-71D4-4F94-AB27-4B5CFC803F5C}">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -68349,8 +68349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -69955,8 +69955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -71003,7 +71003,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>